<commit_message>
OffDays workbook has been made
OffDays workbook has been made
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Website/Antech/UAT-DefectReport-BusinessSite.xlsx
+++ b/Offline/BusinessManagement/Website/Antech/UAT-DefectReport-BusinessSite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Website\Antech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625BDF24-DBA1-4DDA-8D3C-C8F54B639896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB968F2A-4F7B-4BE9-B88A-87F126C30B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Created By</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>1. Visit: https://sites.google.com/view/anodiam</t>
+  </si>
+  <si>
+    <t>Home Page: Body</t>
+  </si>
+  <si>
+    <t>Delete the section as it is not required.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -558,6 +564,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,6 +1129,136 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1424940</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>525780</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{578094E4-762B-A83B-4687-FB47562487DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9715500" y="6332220"/>
+          <a:ext cx="1310640" cy="502920"/>
+          <a:chOff x="0" y="0"/>
+          <a:chExt cx="2298700" cy="937260"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="Picture 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D16D060-AB50-2E08-FE30-986B2C828853}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="2298700" cy="937260"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BDEDF53-915E-8688-EC12-51638BECDA0E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1000125" y="600075"/>
+            <a:ext cx="373380" cy="213360"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1470,7 +1609,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,19 +1827,29 @@
       <c r="J8" s="16"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="19">
         <v>7</v>
       </c>
       <c r="C9" s="15">
         <v>45324</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="D9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="17">
+        <v>5</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="H9" s="17"/>
-      <c r="I9" s="16"/>
+      <c r="I9" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="J9" s="16"/>
       <c r="K9" s="20"/>
     </row>
@@ -2462,6 +2611,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>